<commit_message>
Updated Documentation and added some files (Javadoc is not finished)
</commit_message>
<xml_diff>
--- a/doc/FunktionenTabelle.xlsx
+++ b/doc/FunktionenTabelle.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Funktion</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Guidlines folgen (laut Angabe)</t>
+  </si>
+  <si>
+    <t>Unit-Testing</t>
   </si>
 </sst>
 </file>
@@ -403,13 +406,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -427,47 +427,51 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="20" fontId="6" fillId="7" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="6" fillId="7" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="6" fillId="7" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="6" fillId="7" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="6" fillId="7" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="6" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
@@ -761,7 +765,7 @@
   <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="B2:H14"/>
+      <selection activeCell="B2" sqref="B2:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,270 +781,272 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="18" t="s">
+      <c r="F2" s="33"/>
+      <c r="G2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="34"/>
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="2:8" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24">
+      <c r="C5" s="36"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="18">
         <f>SUM(E6:E7)</f>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="19">
         <f>SUM(F6:F7)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F6" s="9">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="9">
+      <c r="G6" s="15"/>
+      <c r="H6" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="8">
         <v>1</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D7" s="8">
         <v>1</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E7" s="9">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F6" s="10">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
-      <c r="D7" s="9">
-        <v>1</v>
-      </c>
-      <c r="E7" s="10">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F7" s="10">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="15" t="s">
+      <c r="F7" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24">
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="18">
         <f>SUM(E9:E11)</f>
         <v>0.20833333333333331</v>
       </c>
-      <c r="F8" s="25">
-        <f>SUM(F9:F11)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26" t="s">
+      <c r="F8" s="19">
+        <f>SUM(F9,F10,F11,F12)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>2</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10">
+      <c r="D9" s="8"/>
+      <c r="E9" s="9">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F9" s="10">
-        <v>0</v>
-      </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="15" t="s">
+      <c r="F9" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>1</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10">
+      <c r="D10" s="8"/>
+      <c r="E10" s="9">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F10" s="10">
-        <v>0</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="15" t="s">
+      <c r="F10" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>3</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10">
+      <c r="D11" s="8"/>
+      <c r="E11" s="9">
         <v>0.10416666666666667</v>
       </c>
-      <c r="F11" s="10">
-        <v>0</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="15" t="s">
+      <c r="F11" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="13"/>
+      <c r="B12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="35">
+      <c r="C13" s="30"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="23">
         <v>0.25</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="36">
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="24">
         <f>SUM(E5:E11)</f>
         <v>0.49999999999999994</v>
       </c>
-      <c r="F14" s="37">
-        <f>SUM(F5:F13)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="F14" s="25">
+        <f>SUM(F5,F8,F13)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H20" s="5"/>
+      <c r="H20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>